<commit_message>
Updated Project 3 and added Lab 9 files
</commit_message>
<xml_diff>
--- a/Homework/Project_3_Folder/Project3_Part1.xlsx
+++ b/Homework/Project_3_Folder/Project3_Part1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETE4990\homeworkfolder-bryandelion\Homework\Project_3_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E480D39-8689-4BB1-A885-A1E5226DAB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2904B96-2326-4D75-AE39-4FDC6971354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3D150B4-CDAE-444D-96C2-31EA07BFEE5A}"/>
   </bookViews>
@@ -88,9 +88,6 @@
 so that you can avoid players accidently using items</t>
   </si>
   <si>
-    <t>add user feedback, I can see how lacking a promt here would make the UX tougher for less tech players, in other words add -----print(f"You do not meet the requirements to equip {item['name']}.")</t>
-  </si>
-  <si>
     <t>I think this early on you could use a method of detecting future class mismathces or broken/ damaged logic early, I was able to find some logic that adds logging or error raises, add the following just afer 137ln
 if type(player) not in primary_stats:
 logging.warning(f"Unknown class: {type(player).name}")</t>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">general comment on two functions, snippets of utilization </t>
+  </si>
+  <si>
+    <t>add user feedback, I can see how lacking a promt here would make the UX tougher for less tech players, in other words add (f"You do not meet the requirements to equip {item['name']}.")</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088D717E-5E6E-4C38-BCDB-3FC557C32C1A}">
   <dimension ref="F2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="6:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="6:10" ht="144" x14ac:dyDescent="0.3">
@@ -1361,12 +1361,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="6:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="6:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="F5" s="3">
         <v>3</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="6:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
@@ -1374,7 +1374,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="6:10" x14ac:dyDescent="0.3">
@@ -1445,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A60C9E-9415-4B98-86B2-87B20FCE28F3}">
   <dimension ref="F2:I19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F10"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="6:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="6:9" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1480,7 +1480,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="6:9" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1488,7 +1488,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="6:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -1496,10 +1496,10 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="6:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -1507,7 +1507,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="6:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1515,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="6:9" ht="72" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="6:9" x14ac:dyDescent="0.3">
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0054B90B-019C-42B4-8A67-022D664E5B0D}">
   <dimension ref="G3:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="7:10" ht="228.6" x14ac:dyDescent="0.3">
@@ -1608,7 +1608,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="7:10" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1616,10 +1616,10 @@
         <v>3</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
         <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="7:10" ht="319.8" x14ac:dyDescent="0.3">
@@ -1627,7 +1627,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="7:10" ht="409.6" x14ac:dyDescent="0.3">
@@ -1635,10 +1635,10 @@
         <v>5</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="7:10" x14ac:dyDescent="0.3">

</xml_diff>